<commit_message>
fix asyc call run_lobook
</commit_message>
<xml_diff>
--- a/kniha_jazd_ai_11_2025.xlsx
+++ b/kniha_jazd_ai_11_2025.xlsx
@@ -516,17 +516,17 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Vrbové</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
           <t>15:00</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>Vrbové</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>16:00</t>
         </is>
       </c>
       <c r="F3" t="n">
@@ -582,7 +582,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>16:00</t>
+          <t>15:45</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -592,7 +592,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>17:00</t>
+          <t>16:45</t>
         </is>
       </c>
       <c r="F5" t="n">
@@ -648,7 +648,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>15:30</t>
+          <t>15:15</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -658,7 +658,7 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>16:30</t>
+          <t>16:15</t>
         </is>
       </c>
       <c r="F7" t="n">
@@ -912,7 +912,7 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>16:30</t>
+          <t>16:00</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -922,7 +922,7 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>17:30</t>
+          <t>17:00</t>
         </is>
       </c>
       <c r="F15" t="n">

</xml_diff>

<commit_message>
fix odometer final state = state is final after run
</commit_message>
<xml_diff>
--- a/kniha_jazd_ai_11_2025.xlsx
+++ b/kniha_jazd_ai_11_2025.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -473,7 +473,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2025-11-04</t>
+          <t>2025-11-03</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -483,40 +483,40 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>06:30</t>
+          <t>07:00</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Trnava</t>
+          <t>Bratislava</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>07:30</t>
+          <t>08:00</t>
         </is>
       </c>
       <c r="F2" t="n">
-        <v>125654</v>
+        <v>125746</v>
       </c>
       <c r="G2" t="n">
-        <v>47.9</v>
+        <v>92.5</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2025-11-04</t>
+          <t>2025-11-03</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Trnava</t>
+          <t>Bratislava</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>14:00</t>
+          <t>15:30</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -526,20 +526,20 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>15:00</t>
+          <t>16:30</t>
         </is>
       </c>
       <c r="F3" t="n">
-        <v>125701</v>
+        <v>125839</v>
       </c>
       <c r="G3" t="n">
-        <v>47.9</v>
+        <v>92.5</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2025-11-05</t>
+          <t>2025-11-04</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -549,40 +549,40 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>07:15</t>
+          <t>06:30</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Nitra</t>
+          <t>Trnava</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>08:15</t>
+          <t>07:30</t>
         </is>
       </c>
       <c r="F4" t="n">
-        <v>125749</v>
+        <v>125886</v>
       </c>
       <c r="G4" t="n">
-        <v>59.6</v>
+        <v>47.9</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2025-11-05</t>
+          <t>2025-11-04</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Nitra</t>
+          <t>Trnava</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>15:45</t>
+          <t>14:00</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -592,20 +592,20 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>16:45</t>
+          <t>15:00</t>
         </is>
       </c>
       <c r="F5" t="n">
-        <v>125809</v>
+        <v>125934</v>
       </c>
       <c r="G5" t="n">
-        <v>59.6</v>
+        <v>47.9</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2025-11-06</t>
+          <t>2025-11-05</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -620,7 +620,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Trenčín</t>
+          <t>Žilina</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -629,26 +629,26 @@
         </is>
       </c>
       <c r="F6" t="n">
-        <v>125869</v>
+        <v>126060</v>
       </c>
       <c r="G6" t="n">
-        <v>55.9</v>
+        <v>126.1</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2025-11-06</t>
+          <t>2025-11-05</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Trenčín</t>
+          <t>Žilina</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>15:15</t>
+          <t>17:00</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -658,14 +658,14 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>16:15</t>
+          <t>18:00</t>
         </is>
       </c>
       <c r="F7" t="n">
-        <v>125924</v>
+        <v>126187</v>
       </c>
       <c r="G7" t="n">
-        <v>55.9</v>
+        <v>126.1</v>
       </c>
     </row>
     <row r="8">
@@ -681,24 +681,24 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
+          <t>06:00</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Trenčín</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
           <t>07:00</t>
         </is>
       </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>Žilina</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>08:00</t>
-        </is>
-      </c>
       <c r="F8" t="n">
-        <v>125980</v>
+        <v>126242</v>
       </c>
       <c r="G8" t="n">
-        <v>126.1</v>
+        <v>55.9</v>
       </c>
     </row>
     <row r="9">
@@ -709,12 +709,12 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Žilina</t>
+          <t>Trenčín</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>17:00</t>
+          <t>14:30</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -724,20 +724,20 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>18:00</t>
+          <t>15:30</t>
         </is>
       </c>
       <c r="F9" t="n">
-        <v>126106</v>
+        <v>126298</v>
       </c>
       <c r="G9" t="n">
-        <v>126.1</v>
+        <v>55.9</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2025-11-10</t>
+          <t>2025-11-11</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -747,40 +747,40 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>06:00</t>
+          <t>06:15</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Banská Bystrica</t>
+          <t>Bratislava</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>07:00</t>
+          <t>07:15</t>
         </is>
       </c>
       <c r="F10" t="n">
-        <v>126233</v>
+        <v>126391</v>
       </c>
       <c r="G10" t="n">
-        <v>202.7</v>
+        <v>92.5</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2025-11-10</t>
+          <t>2025-11-11</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Banská Bystrica</t>
+          <t>Bratislava</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>18:00</t>
+          <t>14:45</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -790,20 +790,20 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>19:00</t>
+          <t>15:45</t>
         </is>
       </c>
       <c r="F11" t="n">
-        <v>126435</v>
+        <v>126483</v>
       </c>
       <c r="G11" t="n">
-        <v>202.7</v>
+        <v>92.5</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2025-11-11</t>
+          <t>2025-11-12</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -813,40 +813,40 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>06:30</t>
+          <t>07:00</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Zvolen</t>
+          <t>Trnava</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>07:30</t>
+          <t>08:00</t>
         </is>
       </c>
       <c r="F12" t="n">
-        <v>126638</v>
+        <v>126531</v>
       </c>
       <c r="G12" t="n">
-        <v>187</v>
+        <v>47.9</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2025-11-11</t>
+          <t>2025-11-12</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Zvolen</t>
+          <t>Trnava</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>17:30</t>
+          <t>15:00</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -856,20 +856,20 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>18:30</t>
+          <t>16:00</t>
         </is>
       </c>
       <c r="F13" t="n">
-        <v>126825</v>
+        <v>126579</v>
       </c>
       <c r="G13" t="n">
-        <v>187</v>
+        <v>47.9</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2025-11-12</t>
+          <t>2025-11-13</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -879,57 +879,189 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>07:00</t>
+          <t>06:30</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Prievidza</t>
+          <t>Žilina</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>08:00</t>
+          <t>07:30</t>
         </is>
       </c>
       <c r="F14" t="n">
-        <v>127012</v>
+        <v>126705</v>
       </c>
       <c r="G14" t="n">
-        <v>116.4</v>
+        <v>126.1</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>2025-11-12</t>
+          <t>2025-11-13</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Prievidza</t>
+          <t>Žilina</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
+          <t>17:00</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>Vrbové</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>18:00</t>
+        </is>
+      </c>
+      <c r="F15" t="n">
+        <v>126831</v>
+      </c>
+      <c r="G15" t="n">
+        <v>126.1</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>2025-11-14</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Vrbové</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>07:00</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>Banská Bystrica</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>08:00</t>
+        </is>
+      </c>
+      <c r="F16" t="n">
+        <v>127034</v>
+      </c>
+      <c r="G16" t="n">
+        <v>202.7</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>2025-11-14</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Banská Bystrica</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>18:00</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>Vrbové</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>19:00</t>
+        </is>
+      </c>
+      <c r="F17" t="n">
+        <v>127237</v>
+      </c>
+      <c r="G17" t="n">
+        <v>202.7</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>2025-11-28</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Vrbové</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>Servisná Jazda (doladenie)</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>15:00</t>
+        </is>
+      </c>
+      <c r="F18" t="n">
+        <v>127240</v>
+      </c>
+      <c r="G18" t="n">
+        <v>2.9</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>2025-11-28</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Servisná Jazda (doladenie)</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>15:00</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>Vrbové</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
           <t>16:00</t>
         </is>
       </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>Vrbové</t>
-        </is>
-      </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>17:00</t>
-        </is>
-      </c>
-      <c r="F15" t="n">
-        <v>127128</v>
-      </c>
-      <c r="G15" t="n">
-        <v>116.4</v>
+      <c r="F19" t="n">
+        <v>127242</v>
+      </c>
+      <c r="G19" t="n">
+        <v>2.9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add db cache, add calculate km to web page new css responsive
</commit_message>
<xml_diff>
--- a/kniha_jazd_ai_11_2025.xlsx
+++ b/kniha_jazd_ai_11_2025.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G19"/>
+  <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -461,10 +461,15 @@
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
+          <t>Popis Cesty</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
           <t>Stav Tachometra</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>Km Jazda</t>
         </is>
@@ -496,11 +501,16 @@
           <t>08:00</t>
         </is>
       </c>
-      <c r="F2" t="n">
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Obchodné rokovanie o IT</t>
+        </is>
+      </c>
+      <c r="G2" t="n">
         <v>125746</v>
       </c>
-      <c r="G2" t="n">
-        <v>92.5</v>
+      <c r="H2" t="n">
+        <v>92</v>
       </c>
     </row>
     <row r="3">
@@ -529,11 +539,16 @@
           <t>16:30</t>
         </is>
       </c>
-      <c r="F3" t="n">
-        <v>125839</v>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Obchodné rokovanie o IT</t>
+        </is>
       </c>
       <c r="G3" t="n">
-        <v>92.5</v>
+        <v>125838</v>
+      </c>
+      <c r="H3" t="n">
+        <v>92</v>
       </c>
     </row>
     <row r="4">
@@ -562,11 +577,16 @@
           <t>07:30</t>
         </is>
       </c>
-      <c r="F4" t="n">
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Kontrola technického vybavenia</t>
+        </is>
+      </c>
+      <c r="G4" t="n">
         <v>125886</v>
       </c>
-      <c r="G4" t="n">
-        <v>47.9</v>
+      <c r="H4" t="n">
+        <v>48</v>
       </c>
     </row>
     <row r="5">
@@ -582,7 +602,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>14:00</t>
+          <t>15:00</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -592,14 +612,19 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>15:00</t>
-        </is>
-      </c>
-      <c r="F5" t="n">
+          <t>16:00</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>Kontrola technického vybavenia</t>
+        </is>
+      </c>
+      <c r="G5" t="n">
         <v>125934</v>
       </c>
-      <c r="G5" t="n">
-        <v>47.9</v>
+      <c r="H5" t="n">
+        <v>48</v>
       </c>
     </row>
     <row r="6">
@@ -615,24 +640,29 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>06:45</t>
+          <t>07:30</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Žilina</t>
+          <t>Piešťany</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>07:45</t>
-        </is>
-      </c>
-      <c r="F6" t="n">
-        <v>126060</v>
+          <t>08:30</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>Servis IT infraštruktúry</t>
+        </is>
       </c>
       <c r="G6" t="n">
-        <v>126.1</v>
+        <v>125945</v>
+      </c>
+      <c r="H6" t="n">
+        <v>11</v>
       </c>
     </row>
     <row r="7">
@@ -643,35 +673,40 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Žilina</t>
+          <t>Piešťany</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
+          <t>16:00</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Vrbové</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
           <t>17:00</t>
         </is>
       </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>Vrbové</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>18:00</t>
-        </is>
-      </c>
-      <c r="F7" t="n">
-        <v>126187</v>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>Servis IT infraštruktúry</t>
+        </is>
       </c>
       <c r="G7" t="n">
-        <v>126.1</v>
+        <v>125956</v>
+      </c>
+      <c r="H7" t="n">
+        <v>11</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2025-11-07</t>
+          <t>2025-11-06</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -681,40 +716,45 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>06:00</t>
+          <t>06:45</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Trenčín</t>
+          <t>Nitra</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>07:00</t>
-        </is>
-      </c>
-      <c r="F8" t="n">
-        <v>126242</v>
+          <t>07:45</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>Konzultácia vývoja softvéru</t>
+        </is>
       </c>
       <c r="G8" t="n">
-        <v>55.9</v>
+        <v>126016</v>
+      </c>
+      <c r="H8" t="n">
+        <v>60</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2025-11-07</t>
+          <t>2025-11-06</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Trenčín</t>
+          <t>Nitra</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>14:30</t>
+          <t>15:15</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -724,20 +764,25 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>15:30</t>
-        </is>
-      </c>
-      <c r="F9" t="n">
-        <v>126298</v>
+          <t>16:15</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>Konzultácia vývoja softvéru</t>
+        </is>
       </c>
       <c r="G9" t="n">
-        <v>55.9</v>
+        <v>126076</v>
+      </c>
+      <c r="H9" t="n">
+        <v>60</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2025-11-11</t>
+          <t>2025-11-07</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -747,40 +792,45 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>06:15</t>
+          <t>07:15</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Bratislava</t>
+          <t>Trenčín</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>07:15</t>
-        </is>
-      </c>
-      <c r="F10" t="n">
-        <v>126391</v>
+          <t>08:15</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>Implementácia cloud riešenia</t>
+        </is>
       </c>
       <c r="G10" t="n">
-        <v>92.5</v>
+        <v>126132</v>
+      </c>
+      <c r="H10" t="n">
+        <v>56</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2025-11-11</t>
+          <t>2025-11-07</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Bratislava</t>
+          <t>Trenčín</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>14:45</t>
+          <t>16:00</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -790,20 +840,25 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>15:45</t>
-        </is>
-      </c>
-      <c r="F11" t="n">
-        <v>126483</v>
+          <t>17:00</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>Implementácia cloud riešenia</t>
+        </is>
       </c>
       <c r="G11" t="n">
-        <v>92.5</v>
+        <v>126188</v>
+      </c>
+      <c r="H11" t="n">
+        <v>56</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2025-11-12</t>
+          <t>2025-11-10</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -813,40 +868,45 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
+          <t>06:00</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Žilina</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
           <t>07:00</t>
         </is>
       </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>Trnava</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>08:00</t>
-        </is>
-      </c>
-      <c r="F12" t="n">
-        <v>126531</v>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>Analýza bezpečnostných rizík</t>
+        </is>
       </c>
       <c r="G12" t="n">
-        <v>47.9</v>
+        <v>126314</v>
+      </c>
+      <c r="H12" t="n">
+        <v>126</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2025-11-12</t>
+          <t>2025-11-10</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Trnava</t>
+          <t>Žilina</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>15:00</t>
+          <t>17:00</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -856,20 +916,25 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>16:00</t>
-        </is>
-      </c>
-      <c r="F13" t="n">
-        <v>126579</v>
+          <t>18:00</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>Analýza bezpečnostných rizík</t>
+        </is>
       </c>
       <c r="G13" t="n">
-        <v>47.9</v>
+        <v>126440</v>
+      </c>
+      <c r="H13" t="n">
+        <v>126</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2025-11-13</t>
+          <t>2025-11-11</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -884,7 +949,7 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Žilina</t>
+          <t>Banská Bystrica</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
@@ -892,27 +957,32 @@
           <t>07:30</t>
         </is>
       </c>
-      <c r="F14" t="n">
-        <v>126705</v>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>Obchodné rokovanie o IT</t>
+        </is>
       </c>
       <c r="G14" t="n">
-        <v>126.1</v>
+        <v>126642</v>
+      </c>
+      <c r="H14" t="n">
+        <v>202</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>2025-11-13</t>
+          <t>2025-11-11</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Žilina</t>
+          <t>Banská Bystrica</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>17:00</t>
+          <t>18:00</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -922,20 +992,25 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>18:00</t>
-        </is>
-      </c>
-      <c r="F15" t="n">
-        <v>126831</v>
+          <t>19:00</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>Obchodné rokovanie o IT</t>
+        </is>
       </c>
       <c r="G15" t="n">
-        <v>126.1</v>
+        <v>126844</v>
+      </c>
+      <c r="H15" t="n">
+        <v>202</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>2025-11-14</t>
+          <t>2025-11-12</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -950,7 +1025,7 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Banská Bystrica</t>
+          <t>Martin</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
@@ -958,27 +1033,32 @@
           <t>08:00</t>
         </is>
       </c>
-      <c r="F16" t="n">
-        <v>127034</v>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>Kontrola technického vybavenia</t>
+        </is>
       </c>
       <c r="G16" t="n">
-        <v>202.7</v>
+        <v>126928</v>
+      </c>
+      <c r="H16" t="n">
+        <v>84</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>2025-11-14</t>
+          <t>2025-11-12</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Banská Bystrica</t>
+          <t>Martin</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>18:00</t>
+          <t>16:00</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
@@ -988,20 +1068,25 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>19:00</t>
-        </is>
-      </c>
-      <c r="F17" t="n">
-        <v>127237</v>
+          <t>17:00</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>Kontrola technického vybavenia</t>
+        </is>
       </c>
       <c r="G17" t="n">
-        <v>202.7</v>
+        <v>127012</v>
+      </c>
+      <c r="H17" t="n">
+        <v>84</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>2025-11-28</t>
+          <t>2025-11-14</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -1011,40 +1096,45 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>14:00</t>
+          <t>07:00</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Servisná Jazda (doladenie)</t>
+          <t>Prievidza</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>15:00</t>
-        </is>
-      </c>
-      <c r="F18" t="n">
-        <v>127240</v>
+          <t>08:00</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>Konzultácia vývoja softvéru</t>
+        </is>
       </c>
       <c r="G18" t="n">
-        <v>2.9</v>
+        <v>127128</v>
+      </c>
+      <c r="H18" t="n">
+        <v>116</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>2025-11-28</t>
+          <t>2025-11-14</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Servisná Jazda (doladenie)</t>
+          <t>Prievidza</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>15:00</t>
+          <t>16:30</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
@@ -1054,14 +1144,19 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>16:00</t>
-        </is>
-      </c>
-      <c r="F19" t="n">
-        <v>127242</v>
+          <t>17:30</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>Konzultácia vývoja softvéru</t>
+        </is>
       </c>
       <c r="G19" t="n">
-        <v>2.9</v>
+        <v>127244</v>
+      </c>
+      <c r="H19" t="n">
+        <v>116</v>
       </c>
     </row>
   </sheetData>

</xml_diff>